<commit_message>
Glossary-optional , 'Execute' for calling rules
</commit_message>
<xml_diff>
--- a/SubacuteExtract.xlsx
+++ b/SubacuteExtract.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/pyDMNrules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:40009_{2051CD12-E82E-4C9E-8519-88736FC3A225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A371C741-2D8A-4BEC-8C33-9E6EEA956ED3}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:40009_{2051CD12-E82E-4C9E-8519-88736FC3A225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C9A3FC-060A-492A-B99D-444CF9D1AFE0}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SubacuteExtract" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SubacuteExtract!$A$1:$AI$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>UR9910445</t>
   </si>
@@ -90,9 +93,6 @@
     <t>RUG-ADL</t>
   </si>
   <si>
-    <t>Phase Start Date</t>
-  </si>
-  <si>
     <t>FIM Motor score</t>
   </si>
   <si>
@@ -157,13 +157,70 @@
   </si>
   <si>
     <t>4BD2</t>
+  </si>
+  <si>
+    <t>Episode Start Date</t>
+  </si>
+  <si>
+    <t>Expected NWAU21</t>
+  </si>
+  <si>
+    <t>Dialysis Flag</t>
+  </si>
+  <si>
+    <t>Hospital Remoteness</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>3152</t>
+  </si>
+  <si>
+    <t>3166</t>
+  </si>
+  <si>
+    <t>3130</t>
+  </si>
+  <si>
+    <t>3015</t>
+  </si>
+  <si>
+    <t>3045</t>
+  </si>
+  <si>
+    <t>3023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>SA2</t>
+  </si>
+  <si>
+    <t>Indigenous Status</t>
+  </si>
+  <si>
+    <t>Funding Source</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>RadioTherapy Flag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +351,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,12 +703,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1003,28 +1069,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.68359375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.3125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7890625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.20703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.62890625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.3125" style="1" bestFit="1" customWidth="1"/>
@@ -1036,18 +1102,28 @@
     <col min="23" max="23" width="18.62890625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.1015625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.83984375" style="1"/>
+    <col min="26" max="26" width="23.734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.05078125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
@@ -1059,67 +1135,94 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>36</v>
+      <c r="AA1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,12 +1262,35 @@
       <c r="X2" s="1">
         <v>0</v>
       </c>
-      <c r="Z2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC2"/>
+      <c r="Z2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>3.3919999999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1204,12 +1330,35 @@
       <c r="X3" s="1">
         <v>18</v>
       </c>
-      <c r="Z3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3"/>
+      <c r="Z3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>0.54649999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1235,7 +1384,7 @@
         <v>48</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1">
         <v>74</v>
@@ -1252,12 +1401,35 @@
       <c r="X4" s="1">
         <v>0</v>
       </c>
-      <c r="Z4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4"/>
+      <c r="Z4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>2.8342999999999998</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1297,17 +1469,43 @@
       <c r="X5" s="1">
         <v>15</v>
       </c>
-      <c r="Z5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5"/>
+      <c r="Z5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>0.45989999999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>42749</v>
+        <v>42747</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -1342,17 +1540,43 @@
       <c r="X6" s="1">
         <v>18</v>
       </c>
-      <c r="Z6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC6"/>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>0.45889999999999997</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>42750</v>
+        <v>42747</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -1387,12 +1611,37 @@
       <c r="X7" s="1">
         <v>18</v>
       </c>
-      <c r="Z7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC7"/>
+      <c r="Z7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>0.54649999999999999</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>